<commit_message>
Last update from John!
</commit_message>
<xml_diff>
--- a/AeroQuad/isrSerialICD.xlsx
+++ b/AeroQuad/isrSerialICD.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="18105" windowHeight="11595"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>SendSerialTelem</t>
   </si>
@@ -231,6 +231,9 @@
     <t>Send Receiver Commands 1 thru 5</t>
   </si>
   <si>
+    <t>Send Motor Commands 1 thru LASTMOTOR</t>
+  </si>
+  <si>
     <t>Send Motor Axis Commands</t>
   </si>
   <si>
@@ -264,29 +267,23 @@
     <t>Turn Off ESC Calibration/Individual Motor Commands</t>
   </si>
   <si>
-    <t xml:space="preserve">Send Software Motor Commands </t>
-  </si>
-  <si>
-    <t>Send Hardware Motor Commands</t>
-  </si>
-  <si>
-    <t>!</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Send Flight Software Version</t>
-  </si>
-  <si>
-    <t>Send Flight Software Configuration</t>
+    <t>Accel calibration values</t>
+  </si>
+  <si>
+    <t>Send raw accel values</t>
+  </si>
+  <si>
+    <t>Send calibration values</t>
+  </si>
+  <si>
+    <t>Send Bias Compensated Rate Gyros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +427,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -464,6 +462,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -639,21 +638,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D20" sqref="D20:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -668,7 +667,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -682,7 +681,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -696,7 +695,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -710,7 +709,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -724,7 +723,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,7 +737,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -752,7 +751,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -766,7 +765,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -778,7 +777,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -792,7 +791,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -804,12 +803,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -818,19 +817,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="D13" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -839,10 +840,10 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -851,22 +852,24 @@
         <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -874,9 +877,11 @@
       <c r="C17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -886,7 +891,7 @@
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -898,7 +903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -908,7 +913,7 @@
       </c>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -918,7 +923,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -928,7 +933,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -938,7 +943,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -950,11 +955,13 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>52</v>
       </c>
@@ -962,7 +969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -972,7 +979,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -981,114 +988,100 @@
         <v>54</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
+      </c>
+      <c r="C28" s="2">
+        <v>6</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="2">
-        <v>6</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>77</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>5</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1097,24 +1090,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>